<commit_message>
updated datasets and scripts
</commit_message>
<xml_diff>
--- a/optics.sample.log.ALL.xlsx
+++ b/optics.sample.log.ALL.xlsx
@@ -1544,9 +1544,9 @@
   <dimension ref="A1:J156"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1800" topLeftCell="A133" activePane="bottomLeft"/>
+      <pane ySplit="1800" topLeftCell="A124" activePane="bottomLeft"/>
       <selection activeCell="D3" sqref="D3"/>
-      <selection pane="bottomLeft" activeCell="D135" sqref="D135"/>
+      <selection pane="bottomLeft" activeCell="D146" sqref="D146"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2517,7 +2517,7 @@
         <v>2</v>
       </c>
       <c r="D34" s="26" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="E34" s="28">
         <v>41649.697916666664</v>
@@ -2691,7 +2691,7 @@
         <v>2</v>
       </c>
       <c r="D40" s="26" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="E40" s="28">
         <v>41886.21875</v>
@@ -2720,7 +2720,7 @@
         <v>5</v>
       </c>
       <c r="D41" s="26" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="E41" s="28">
         <v>41886.8125</v>
@@ -4089,7 +4089,7 @@
         <v>2</v>
       </c>
       <c r="D89" s="26" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="E89" s="28">
         <v>41886.213194444441</v>
@@ -4549,7 +4549,7 @@
         <v>2</v>
       </c>
       <c r="D105" s="26" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="E105" s="28">
         <v>41886.302083333336</v>
@@ -4578,7 +4578,7 @@
         <v>5</v>
       </c>
       <c r="D106" s="26" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="E106" s="28">
         <v>41886.71875</v>
@@ -5440,7 +5440,7 @@
         <v>5</v>
       </c>
       <c r="D136" s="26" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="E136" s="28">
         <v>41886.802083333336</v>

</xml_diff>